<commit_message>
PAS-6576 fixed VinUpload file for UT SS, changed: Bi symbols value from I to X for valid VIN
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/UpdatedVIN_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/UpdatedVIN_UT_SS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="73">
   <si>
     <t>VIN</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>secondValid</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -604,7 +607,7 @@
   <dimension ref="A1:AL7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1065,16 +1068,16 @@
         <v>39</v>
       </c>
       <c r="AE4" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="AF4" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="AG4" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="AH4" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="AI4" s="5">
         <v>20020101</v>
@@ -1181,16 +1184,16 @@
         <v>39</v>
       </c>
       <c r="AE5" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="AF5" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="AG5" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="AH5" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="AI5" s="5">
         <v>20030101</v>

</xml_diff>